<commit_message>
item excel add count column
</commit_message>
<xml_diff>
--- a/excel_templates/items_template.xlsx
+++ b/excel_templates/items_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ligangzhou/Money/rust/store-api/excel_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{408949AF-359B-5844-B370-D95FAF380AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73FB15C-8FB7-4941-91F2-6D252488D581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="1820" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="产品列表" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>产品大类</t>
   </si>
@@ -137,6 +137,10 @@
   </si>
   <si>
     <t>asd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -579,10 +583,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="ThisWorkbook"/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -591,7 +595,7 @@
     <col min="2" max="253" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -628,8 +632,11 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="284" customHeight="1">
+    <row r="2" spans="1:13" ht="284" customHeight="1">
       <c r="A2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -664,8 +671,11 @@
       <c r="L2">
         <v>0.03</v>
       </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="171" customHeight="1">
+    <row r="3" spans="1:13" ht="171" customHeight="1">
       <c r="A3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -698,6 +708,9 @@
       </c>
       <c r="L3" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="M3">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>